<commit_message>
update bound constraint and add new formulation
</commit_message>
<xml_diff>
--- a/ModeloMatematico.xlsx
+++ b/ModeloMatematico.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgutiea/Desktop/TSPJ_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4162D617-031F-BC4B-A441-160E61C68A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA5760A-4A5F-964E-A730-DF379A59C91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="760" windowWidth="34380" windowHeight="18100" activeTab="2" xr2:uid="{A1F54B34-08F9-7D4B-B42D-D2E4DC4AEBFC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{A1F54B34-08F9-7D4B-B42D-D2E4DC4AEBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="trabajos (2)" sheetId="4" r:id="rId2"/>
-    <sheet name="LSJA" sheetId="5" r:id="rId3"/>
-    <sheet name="trabajos" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
+    <sheet name="gr17" sheetId="4" r:id="rId2"/>
+    <sheet name="bays29" sheetId="6" r:id="rId3"/>
+    <sheet name="LSJA" sheetId="5" r:id="rId4"/>
+    <sheet name="trabajos" sheetId="3" r:id="rId5"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId6"/>
+    <sheet name="Hoja3" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">trabajos!$A$1:$C$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'trabajos (2)'!$A$1:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'gr17'!$A$1:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">trabajos!$A$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="61">
   <si>
     <t>objective</t>
   </si>
@@ -205,6 +207,51 @@
   <si>
     <t>cambio_i</t>
   </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>instance</t>
+  </si>
+  <si>
+    <t>obj</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Sol Count</t>
+  </si>
+  <si>
+    <t>NodeCount</t>
+  </si>
+  <si>
+    <t>#callback</t>
+  </si>
+  <si>
+    <t>timecallback</t>
+  </si>
+  <si>
+    <t>tsplib</t>
+  </si>
+  <si>
+    <t>OPTIMAL</t>
+  </si>
+  <si>
+    <t>Formulacion antigua</t>
+  </si>
+  <si>
+    <t>Formulacion nueva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running with parameters: ['secuential', 'tsplib', 'gurobi', 'wc', 'True', 'cut_naive_fractional_separation', 'True', 'True'] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running with parameters: ['secuential', 'tsplib', 'gurobi', 'wc', 'True', 'cut_smarter_fractional_separation', 'True', 'True'] </t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +343,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE699"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -512,7 +565,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -621,6 +674,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -1782,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEAB757-C98E-CE48-A531-62280EF3C31D}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3126,11 +3180,1333 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308CA008-94DA-7B42-907D-0F541B1F3776}">
+  <dimension ref="A1:V51"/>
+  <sheetViews>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="22" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="30">
+        <v>1</v>
+      </c>
+      <c r="H1" s="30">
+        <v>2</v>
+      </c>
+      <c r="I1" s="30">
+        <v>3</v>
+      </c>
+      <c r="J1" s="30">
+        <v>4</v>
+      </c>
+      <c r="K1">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>6</v>
+      </c>
+      <c r="M1" s="30">
+        <v>7</v>
+      </c>
+      <c r="N1" s="30">
+        <v>8</v>
+      </c>
+      <c r="O1">
+        <v>9</v>
+      </c>
+      <c r="P1" s="30">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="30">
+        <v>11</v>
+      </c>
+      <c r="R1">
+        <v>12</v>
+      </c>
+      <c r="S1" s="30">
+        <v>13</v>
+      </c>
+      <c r="T1" s="30">
+        <v>14</v>
+      </c>
+      <c r="U1" s="30">
+        <v>15</v>
+      </c>
+      <c r="V1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0.11845730027548</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="30">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30">
+        <v>0</v>
+      </c>
+      <c r="I2" s="30">
+        <v>0</v>
+      </c>
+      <c r="J2" s="30">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="30">
+        <v>0</v>
+      </c>
+      <c r="N2" s="30">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="30">
+        <v>0</v>
+      </c>
+      <c r="T2" s="30">
+        <v>0</v>
+      </c>
+      <c r="U2" s="30">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0.88154269972451904</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
+        <v>1235</v>
+      </c>
+      <c r="H3" s="30">
+        <v>1661</v>
+      </c>
+      <c r="I3" s="30">
+        <v>1220</v>
+      </c>
+      <c r="J3" s="30">
+        <v>1404</v>
+      </c>
+      <c r="K3">
+        <v>1468</v>
+      </c>
+      <c r="L3">
+        <v>1385</v>
+      </c>
+      <c r="M3" s="30">
+        <v>1053</v>
+      </c>
+      <c r="N3" s="30">
+        <v>1622</v>
+      </c>
+      <c r="O3">
+        <v>1246</v>
+      </c>
+      <c r="P3" s="30">
+        <v>1653</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>1307</v>
+      </c>
+      <c r="R3">
+        <v>1177</v>
+      </c>
+      <c r="S3" s="30">
+        <v>1614</v>
+      </c>
+      <c r="T3" s="30">
+        <v>1313</v>
+      </c>
+      <c r="U3" s="30">
+        <v>1548</v>
+      </c>
+      <c r="V3">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0.88154269972451904</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <v>1334</v>
+      </c>
+      <c r="H4" s="30">
+        <v>1315</v>
+      </c>
+      <c r="I4" s="30">
+        <v>1354</v>
+      </c>
+      <c r="J4" s="30">
+        <v>1289</v>
+      </c>
+      <c r="K4">
+        <v>1064</v>
+      </c>
+      <c r="L4">
+        <v>1315</v>
+      </c>
+      <c r="M4" s="30">
+        <v>1453</v>
+      </c>
+      <c r="N4" s="30">
+        <v>1463</v>
+      </c>
+      <c r="O4">
+        <v>1144</v>
+      </c>
+      <c r="P4" s="30">
+        <v>1059</v>
+      </c>
+      <c r="Q4" s="31">
+        <v>1043</v>
+      </c>
+      <c r="R4">
+        <v>1540</v>
+      </c>
+      <c r="S4" s="30">
+        <v>1533</v>
+      </c>
+      <c r="T4" s="30">
+        <v>1631</v>
+      </c>
+      <c r="U4" s="30">
+        <v>1127</v>
+      </c>
+      <c r="V4">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0.11845730027548</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>1219</v>
+      </c>
+      <c r="H5" s="30">
+        <v>1656</v>
+      </c>
+      <c r="I5" s="30">
+        <v>1486</v>
+      </c>
+      <c r="J5" s="30">
+        <v>1414</v>
+      </c>
+      <c r="K5">
+        <v>1242</v>
+      </c>
+      <c r="L5">
+        <v>1201</v>
+      </c>
+      <c r="M5" s="30">
+        <v>1203</v>
+      </c>
+      <c r="N5" s="30">
+        <v>1204</v>
+      </c>
+      <c r="O5">
+        <v>1586</v>
+      </c>
+      <c r="P5" s="30">
+        <v>1362</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>1547</v>
+      </c>
+      <c r="R5">
+        <v>1207</v>
+      </c>
+      <c r="S5" s="30">
+        <v>1494</v>
+      </c>
+      <c r="T5" s="30">
+        <v>1399</v>
+      </c>
+      <c r="U5" s="30">
+        <v>1580</v>
+      </c>
+      <c r="V5">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="28">
+        <v>0.11845730027548</v>
+      </c>
+      <c r="E6" s="30">
+        <v>4</v>
+      </c>
+      <c r="F6" s="30">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
+        <v>1081</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1545</v>
+      </c>
+      <c r="I6" s="30">
+        <v>1619</v>
+      </c>
+      <c r="J6" s="30">
+        <v>1160</v>
+      </c>
+      <c r="K6" s="30">
+        <v>1435</v>
+      </c>
+      <c r="L6" s="30">
+        <v>1491</v>
+      </c>
+      <c r="M6" s="30">
+        <v>1205</v>
+      </c>
+      <c r="N6">
+        <v>1562</v>
+      </c>
+      <c r="O6" s="30">
+        <v>1138</v>
+      </c>
+      <c r="P6" s="30">
+        <v>1486</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>1178</v>
+      </c>
+      <c r="R6" s="30">
+        <v>1137</v>
+      </c>
+      <c r="S6" s="30">
+        <v>1628</v>
+      </c>
+      <c r="T6" s="30">
+        <v>1379</v>
+      </c>
+      <c r="U6" s="30">
+        <v>1261</v>
+      </c>
+      <c r="V6" s="30">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="28">
+        <v>0.88154269972451904</v>
+      </c>
+      <c r="E7" s="30">
+        <v>5</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1052</v>
+      </c>
+      <c r="H7" s="30">
+        <v>1044</v>
+      </c>
+      <c r="I7" s="30">
+        <v>1463</v>
+      </c>
+      <c r="J7" s="30">
+        <v>1326</v>
+      </c>
+      <c r="K7" s="30">
+        <v>1292</v>
+      </c>
+      <c r="L7" s="30">
+        <v>1658</v>
+      </c>
+      <c r="M7" s="30">
+        <v>1480</v>
+      </c>
+      <c r="N7" s="30">
+        <v>1578</v>
+      </c>
+      <c r="O7" s="30">
+        <v>1152</v>
+      </c>
+      <c r="P7" s="30">
+        <v>1607</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>1384</v>
+      </c>
+      <c r="R7" s="30">
+        <v>1389</v>
+      </c>
+      <c r="S7" s="30">
+        <v>1449</v>
+      </c>
+      <c r="T7" s="30">
+        <v>1151</v>
+      </c>
+      <c r="U7" s="30">
+        <v>1208</v>
+      </c>
+      <c r="V7" s="30">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29">
+        <v>8</v>
+      </c>
+      <c r="C8" s="28">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30">
+        <v>6</v>
+      </c>
+      <c r="F8" s="30">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
+        <v>1196</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1368</v>
+      </c>
+      <c r="I8" s="30">
+        <v>1548</v>
+      </c>
+      <c r="J8" s="30">
+        <v>1630</v>
+      </c>
+      <c r="K8" s="30">
+        <v>1243</v>
+      </c>
+      <c r="L8" s="30">
+        <v>1465</v>
+      </c>
+      <c r="M8" s="30">
+        <v>1601</v>
+      </c>
+      <c r="N8" s="30">
+        <v>1379</v>
+      </c>
+      <c r="O8" s="30">
+        <v>1560</v>
+      </c>
+      <c r="P8" s="30">
+        <v>1450</v>
+      </c>
+      <c r="Q8">
+        <v>1138</v>
+      </c>
+      <c r="R8" s="30">
+        <v>1356</v>
+      </c>
+      <c r="S8" s="30">
+        <v>1333</v>
+      </c>
+      <c r="T8" s="30">
+        <v>1631</v>
+      </c>
+      <c r="U8" s="30">
+        <v>1604</v>
+      </c>
+      <c r="V8" s="30">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1</v>
+      </c>
+      <c r="E9" s="30">
+        <v>7</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
+        <v>1311</v>
+      </c>
+      <c r="H9" s="30">
+        <v>1241</v>
+      </c>
+      <c r="I9" s="30">
+        <v>1112</v>
+      </c>
+      <c r="J9" s="30">
+        <v>1540</v>
+      </c>
+      <c r="K9" s="30">
+        <v>1408</v>
+      </c>
+      <c r="L9" s="30">
+        <v>1142</v>
+      </c>
+      <c r="M9" s="30">
+        <v>1168</v>
+      </c>
+      <c r="N9" s="30">
+        <v>1366</v>
+      </c>
+      <c r="O9" s="30">
+        <v>1309</v>
+      </c>
+      <c r="P9" s="30">
+        <v>1385</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>1245</v>
+      </c>
+      <c r="R9" s="30">
+        <v>1328</v>
+      </c>
+      <c r="S9">
+        <v>1133</v>
+      </c>
+      <c r="T9" s="30">
+        <v>1546</v>
+      </c>
+      <c r="U9" s="30">
+        <v>1440</v>
+      </c>
+      <c r="V9" s="30">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="29">
+        <v>11</v>
+      </c>
+      <c r="C10" s="28">
+        <v>1</v>
+      </c>
+      <c r="E10" s="30">
+        <v>8</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <v>1239</v>
+      </c>
+      <c r="H10">
+        <v>1047</v>
+      </c>
+      <c r="I10" s="30">
+        <v>1299</v>
+      </c>
+      <c r="J10" s="30">
+        <v>1236</v>
+      </c>
+      <c r="K10" s="30">
+        <v>1301</v>
+      </c>
+      <c r="L10" s="30">
+        <v>1377</v>
+      </c>
+      <c r="M10" s="30">
+        <v>1666</v>
+      </c>
+      <c r="N10" s="30">
+        <v>1423</v>
+      </c>
+      <c r="O10" s="30">
+        <v>1589</v>
+      </c>
+      <c r="P10" s="30">
+        <v>1596</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>1331</v>
+      </c>
+      <c r="R10" s="30">
+        <v>1542</v>
+      </c>
+      <c r="S10" s="30">
+        <v>1329</v>
+      </c>
+      <c r="T10" s="30">
+        <v>1370</v>
+      </c>
+      <c r="U10" s="30">
+        <v>1559</v>
+      </c>
+      <c r="V10" s="30">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29">
+        <v>13</v>
+      </c>
+      <c r="C11" s="28">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="30">
+        <v>1264</v>
+      </c>
+      <c r="H11" s="30">
+        <v>1580</v>
+      </c>
+      <c r="I11" s="30">
+        <v>1326</v>
+      </c>
+      <c r="J11" s="30">
+        <v>1120</v>
+      </c>
+      <c r="K11">
+        <v>1324</v>
+      </c>
+      <c r="L11">
+        <v>1420</v>
+      </c>
+      <c r="M11" s="30">
+        <v>1239</v>
+      </c>
+      <c r="N11" s="30">
+        <v>1626</v>
+      </c>
+      <c r="O11">
+        <v>1211</v>
+      </c>
+      <c r="P11" s="30">
+        <v>1461</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>1648</v>
+      </c>
+      <c r="R11">
+        <v>1200</v>
+      </c>
+      <c r="S11" s="30">
+        <v>1545</v>
+      </c>
+      <c r="T11" s="30">
+        <v>1262</v>
+      </c>
+      <c r="U11" s="30">
+        <v>1439</v>
+      </c>
+      <c r="V11">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29">
+        <v>2</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30">
+        <v>10</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0</v>
+      </c>
+      <c r="G12" s="30">
+        <v>1562</v>
+      </c>
+      <c r="H12" s="30">
+        <v>1584</v>
+      </c>
+      <c r="I12" s="30">
+        <v>1117</v>
+      </c>
+      <c r="J12" s="30">
+        <v>1656</v>
+      </c>
+      <c r="K12" s="30">
+        <v>1529</v>
+      </c>
+      <c r="L12" s="30">
+        <v>1353</v>
+      </c>
+      <c r="M12" s="30">
+        <v>1476</v>
+      </c>
+      <c r="N12" s="30">
+        <v>1422</v>
+      </c>
+      <c r="O12" s="30">
+        <v>1192</v>
+      </c>
+      <c r="P12" s="30">
+        <v>1353</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>1637</v>
+      </c>
+      <c r="R12" s="30">
+        <v>1218</v>
+      </c>
+      <c r="S12" s="30">
+        <v>1125</v>
+      </c>
+      <c r="T12" s="30">
+        <v>1098</v>
+      </c>
+      <c r="U12">
+        <v>1053</v>
+      </c>
+      <c r="V12" s="30">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0.11845730027548</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="30">
+        <v>1378</v>
+      </c>
+      <c r="H13" s="30">
+        <v>1478</v>
+      </c>
+      <c r="I13" s="30">
+        <v>1076</v>
+      </c>
+      <c r="J13" s="30">
+        <v>1131</v>
+      </c>
+      <c r="K13">
+        <v>1472</v>
+      </c>
+      <c r="L13">
+        <v>1050</v>
+      </c>
+      <c r="M13" s="30">
+        <v>1490</v>
+      </c>
+      <c r="N13" s="30">
+        <v>1301</v>
+      </c>
+      <c r="O13" s="32">
+        <v>1045</v>
+      </c>
+      <c r="P13" s="30">
+        <v>1131</v>
+      </c>
+      <c r="Q13" s="30">
+        <v>1641</v>
+      </c>
+      <c r="R13">
+        <v>1292</v>
+      </c>
+      <c r="S13" s="30">
+        <v>1102</v>
+      </c>
+      <c r="T13" s="30">
+        <v>1369</v>
+      </c>
+      <c r="U13" s="30">
+        <v>1399</v>
+      </c>
+      <c r="V13">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0.88154269972451904</v>
+      </c>
+      <c r="E14" s="30">
+        <v>12</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0</v>
+      </c>
+      <c r="G14" s="30">
+        <v>1205</v>
+      </c>
+      <c r="H14" s="30">
+        <v>1188</v>
+      </c>
+      <c r="I14" s="30">
+        <v>1323</v>
+      </c>
+      <c r="J14" s="30">
+        <v>1640</v>
+      </c>
+      <c r="K14" s="30">
+        <v>1372</v>
+      </c>
+      <c r="L14" s="30">
+        <v>1115</v>
+      </c>
+      <c r="M14" s="30">
+        <v>1576</v>
+      </c>
+      <c r="N14" s="30">
+        <v>1504</v>
+      </c>
+      <c r="O14" s="30">
+        <v>1426</v>
+      </c>
+      <c r="P14" s="30">
+        <v>1123</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>1224</v>
+      </c>
+      <c r="R14" s="30">
+        <v>1262</v>
+      </c>
+      <c r="S14" s="30">
+        <v>1385</v>
+      </c>
+      <c r="T14">
+        <v>1063</v>
+      </c>
+      <c r="U14" s="30">
+        <v>1623</v>
+      </c>
+      <c r="V14" s="30">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" s="29">
+        <v>15</v>
+      </c>
+      <c r="C15" s="28">
+        <v>1</v>
+      </c>
+      <c r="E15" s="30">
+        <v>13</v>
+      </c>
+      <c r="F15" s="30">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30">
+        <v>1656</v>
+      </c>
+      <c r="H15" s="30">
+        <v>1166</v>
+      </c>
+      <c r="I15">
+        <v>1296</v>
+      </c>
+      <c r="J15" s="30">
+        <v>1153</v>
+      </c>
+      <c r="K15" s="30">
+        <v>1068</v>
+      </c>
+      <c r="L15" s="30">
+        <v>1294</v>
+      </c>
+      <c r="M15" s="30">
+        <v>1646</v>
+      </c>
+      <c r="N15" s="30">
+        <v>1284</v>
+      </c>
+      <c r="O15" s="30">
+        <v>1197</v>
+      </c>
+      <c r="P15" s="30">
+        <v>1276</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>1215</v>
+      </c>
+      <c r="R15" s="30">
+        <v>1057</v>
+      </c>
+      <c r="S15" s="30">
+        <v>1439</v>
+      </c>
+      <c r="T15" s="30">
+        <v>1212</v>
+      </c>
+      <c r="U15" s="30">
+        <v>1302</v>
+      </c>
+      <c r="V15" s="30">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0.11845730027548</v>
+      </c>
+      <c r="E16" s="30">
+        <v>14</v>
+      </c>
+      <c r="F16" s="30">
+        <v>0</v>
+      </c>
+      <c r="G16" s="30">
+        <v>1242</v>
+      </c>
+      <c r="H16" s="30">
+        <v>1211</v>
+      </c>
+      <c r="I16" s="30">
+        <v>1293</v>
+      </c>
+      <c r="J16" s="30">
+        <v>1607</v>
+      </c>
+      <c r="K16" s="30">
+        <v>1157</v>
+      </c>
+      <c r="L16" s="30">
+        <v>1412</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1210</v>
+      </c>
+      <c r="N16" s="30">
+        <v>1197</v>
+      </c>
+      <c r="O16" s="30">
+        <v>1180</v>
+      </c>
+      <c r="P16">
+        <v>1128</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>1327</v>
+      </c>
+      <c r="R16" s="30">
+        <v>1230</v>
+      </c>
+      <c r="S16" s="30">
+        <v>1172</v>
+      </c>
+      <c r="T16" s="30">
+        <v>1156</v>
+      </c>
+      <c r="U16" s="30">
+        <v>1410</v>
+      </c>
+      <c r="V16" s="30">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0.88154269972451904</v>
+      </c>
+      <c r="E17" s="30">
+        <v>15</v>
+      </c>
+      <c r="F17" s="30">
+        <v>0</v>
+      </c>
+      <c r="G17" s="30">
+        <v>1304</v>
+      </c>
+      <c r="H17" s="30">
+        <v>1370</v>
+      </c>
+      <c r="I17" s="30">
+        <v>1311</v>
+      </c>
+      <c r="J17">
+        <v>1161</v>
+      </c>
+      <c r="K17" s="30">
+        <v>1196</v>
+      </c>
+      <c r="L17" s="30">
+        <v>1394</v>
+      </c>
+      <c r="M17" s="30">
+        <v>1391</v>
+      </c>
+      <c r="N17" s="30">
+        <v>1571</v>
+      </c>
+      <c r="O17" s="30">
+        <v>1381</v>
+      </c>
+      <c r="P17" s="30">
+        <v>1411</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>1325</v>
+      </c>
+      <c r="R17" s="30">
+        <v>1600</v>
+      </c>
+      <c r="S17" s="30">
+        <v>1368</v>
+      </c>
+      <c r="T17" s="30">
+        <v>1227</v>
+      </c>
+      <c r="U17" s="30">
+        <v>1253</v>
+      </c>
+      <c r="V17" s="30">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="29">
+        <v>14</v>
+      </c>
+      <c r="C18" s="28">
+        <v>1</v>
+      </c>
+      <c r="E18" s="30">
+        <v>16</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0</v>
+      </c>
+      <c r="G18" s="30">
+        <v>1266</v>
+      </c>
+      <c r="H18" s="30">
+        <v>1175</v>
+      </c>
+      <c r="I18" s="30">
+        <v>1229</v>
+      </c>
+      <c r="J18" s="30">
+        <v>1372</v>
+      </c>
+      <c r="K18" s="30">
+        <v>1347</v>
+      </c>
+      <c r="L18" s="30">
+        <v>1264</v>
+      </c>
+      <c r="M18">
+        <v>1261</v>
+      </c>
+      <c r="N18" s="30">
+        <v>1620</v>
+      </c>
+      <c r="O18" s="30">
+        <v>1220</v>
+      </c>
+      <c r="P18" s="30">
+        <v>1431</v>
+      </c>
+      <c r="Q18" s="30">
+        <v>1577</v>
+      </c>
+      <c r="R18" s="30">
+        <v>1551</v>
+      </c>
+      <c r="S18" s="30">
+        <v>1358</v>
+      </c>
+      <c r="T18" s="30">
+        <v>1396</v>
+      </c>
+      <c r="U18" s="30">
+        <v>1362</v>
+      </c>
+      <c r="V18" s="30">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="29">
+        <v>3</v>
+      </c>
+      <c r="C19" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" s="29">
+        <v>10</v>
+      </c>
+      <c r="C20" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="29">
+        <v>4</v>
+      </c>
+      <c r="C21" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" s="29">
+        <v>7</v>
+      </c>
+      <c r="C22" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C23" s="28"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C25" s="28"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C28" s="28"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C29" s="28"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C31" s="28"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C32" s="28"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="28"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="28"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="28"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="28"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="28"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="28"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="28"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="28"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="28"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="28"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="28"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="28"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="28"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="28"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="28"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="28"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4FED5A-D8CC-B141-B64A-46BCE3F5BE95}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K32" sqref="C22:R37"/>
+    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3138,7 +4514,8 @@
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -3202,31 +4579,31 @@
       </c>
       <c r="Z1">
         <f>Z8</f>
-        <v>1499</v>
+        <v>1627</v>
       </c>
       <c r="AA1">
         <f t="shared" ref="AA1:AO1" si="0">AA8</f>
-        <v>1448</v>
+        <v>1534</v>
       </c>
       <c r="AB1">
         <f t="shared" si="0"/>
-        <v>1737</v>
+        <v>1545</v>
       </c>
       <c r="AC1">
         <f t="shared" si="0"/>
-        <v>2329</v>
+        <v>2253</v>
       </c>
       <c r="AD1">
         <f t="shared" si="0"/>
-        <v>1823</v>
+        <v>1763</v>
       </c>
       <c r="AE1">
         <f t="shared" si="0"/>
-        <v>2378</v>
+        <v>2295</v>
       </c>
       <c r="AF1">
         <f t="shared" si="0"/>
-        <v>1909</v>
+        <v>2087</v>
       </c>
       <c r="AG1">
         <f t="shared" si="0"/>
@@ -3234,35 +4611,35 @@
       </c>
       <c r="AH1">
         <f t="shared" si="0"/>
-        <v>2217</v>
+        <v>2109</v>
       </c>
       <c r="AI1">
         <f t="shared" si="0"/>
-        <v>2587</v>
+        <v>2009</v>
       </c>
       <c r="AJ1">
         <f t="shared" si="0"/>
-        <v>2410</v>
+        <v>2325</v>
       </c>
       <c r="AK1">
         <f t="shared" si="0"/>
-        <v>2591</v>
+        <v>2514</v>
       </c>
       <c r="AL1">
         <f t="shared" si="0"/>
-        <v>2278</v>
+        <v>2286</v>
       </c>
       <c r="AM1">
         <f t="shared" si="0"/>
-        <v>2784</v>
+        <v>2359</v>
       </c>
       <c r="AN1">
         <f t="shared" si="0"/>
-        <v>3066</v>
+        <v>2538</v>
       </c>
       <c r="AO1">
         <f t="shared" si="0"/>
-        <v>3175</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
@@ -3539,52 +4916,52 @@
         <v>34</v>
       </c>
       <c r="Z4" s="33">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="33">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="33">
         <v>15</v>
       </c>
-      <c r="AA4" s="33">
-        <v>9</v>
-      </c>
-      <c r="AB4" s="33">
+      <c r="AD4" s="33">
+        <v>14</v>
+      </c>
+      <c r="AE4" s="33">
+        <v>3</v>
+      </c>
+      <c r="AF4" s="33">
         <v>1</v>
-      </c>
-      <c r="AC4" s="33">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="33">
-        <v>10</v>
-      </c>
-      <c r="AE4" s="33">
-        <v>14</v>
-      </c>
-      <c r="AF4" s="33">
-        <v>13</v>
       </c>
       <c r="AG4" s="33">
         <v>16</v>
       </c>
       <c r="AH4" s="33">
+        <v>6</v>
+      </c>
+      <c r="AI4" s="33">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="33">
+        <v>11</v>
+      </c>
+      <c r="AK4" s="33">
+        <v>8</v>
+      </c>
+      <c r="AL4" s="33">
+        <v>13</v>
+      </c>
+      <c r="AM4" s="33">
+        <v>12</v>
+      </c>
+      <c r="AN4" s="33">
         <v>4</v>
       </c>
-      <c r="AI4" s="33">
+      <c r="AO4" s="33">
         <v>7</v>
-      </c>
-      <c r="AJ4" s="33">
-        <v>6</v>
-      </c>
-      <c r="AK4" s="33">
-        <v>12</v>
-      </c>
-      <c r="AL4" s="33">
-        <v>3</v>
-      </c>
-      <c r="AM4" s="33">
-        <v>8</v>
-      </c>
-      <c r="AN4" s="33">
-        <v>11</v>
-      </c>
-      <c r="AO4" s="33">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -3893,31 +5270,31 @@
       </c>
       <c r="Z7">
         <f>HLOOKUP(Z4,$A$20:$R$37,Z3+2)</f>
-        <v>1253</v>
+        <v>1381</v>
       </c>
       <c r="AA7">
         <f>HLOOKUP(AA4,$A$20:$R$37,AA3+2)</f>
-        <v>1045</v>
+        <v>1131</v>
       </c>
       <c r="AB7">
-        <f t="shared" ref="AA7:AO7" si="3">HLOOKUP(AB4,$A$20:$R$37,AB3+2)</f>
-        <v>1239</v>
+        <f t="shared" ref="AB7:AO7" si="3">HLOOKUP(AB4,$A$20:$R$37,AB3+2)</f>
+        <v>1047</v>
       </c>
       <c r="AC7">
         <f t="shared" si="3"/>
-        <v>1656</v>
+        <v>1580</v>
       </c>
       <c r="AD7">
         <f t="shared" si="3"/>
-        <v>1123</v>
+        <v>1063</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
-        <v>1631</v>
+        <v>1548</v>
       </c>
       <c r="AF7">
         <f t="shared" si="3"/>
-        <v>1133</v>
+        <v>1311</v>
       </c>
       <c r="AG7">
         <f t="shared" si="3"/>
@@ -3925,35 +5302,35 @@
       </c>
       <c r="AH7">
         <f t="shared" si="3"/>
-        <v>1372</v>
+        <v>1264</v>
       </c>
       <c r="AI7">
         <f t="shared" si="3"/>
-        <v>1646</v>
+        <v>1068</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="3"/>
-        <v>1412</v>
+        <v>1327</v>
       </c>
       <c r="AK7">
         <f t="shared" si="3"/>
-        <v>1540</v>
+        <v>1463</v>
       </c>
       <c r="AL7">
         <f t="shared" si="3"/>
-        <v>1117</v>
+        <v>1125</v>
       </c>
       <c r="AM7">
         <f t="shared" si="3"/>
-        <v>1562</v>
+        <v>1137</v>
       </c>
       <c r="AN7">
         <f t="shared" si="3"/>
-        <v>1648</v>
+        <v>1120</v>
       </c>
       <c r="AO7">
         <f t="shared" si="3"/>
-        <v>1468</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.2">
@@ -4016,31 +5393,31 @@
       </c>
       <c r="Z8">
         <f>Z6+Z7</f>
-        <v>1499</v>
+        <v>1627</v>
       </c>
       <c r="AA8">
         <f t="shared" ref="AA8:AO8" si="4">AA6+AA7</f>
-        <v>1448</v>
+        <v>1534</v>
       </c>
       <c r="AB8">
         <f t="shared" si="4"/>
-        <v>1737</v>
+        <v>1545</v>
       </c>
       <c r="AC8">
         <f t="shared" si="4"/>
-        <v>2329</v>
+        <v>2253</v>
       </c>
       <c r="AD8">
         <f t="shared" si="4"/>
-        <v>1823</v>
+        <v>1763</v>
       </c>
       <c r="AE8">
         <f t="shared" si="4"/>
-        <v>2378</v>
+        <v>2295</v>
       </c>
       <c r="AF8">
         <f t="shared" si="4"/>
-        <v>1909</v>
+        <v>2087</v>
       </c>
       <c r="AG8">
         <f t="shared" si="4"/>
@@ -4048,35 +5425,35 @@
       </c>
       <c r="AH8">
         <f t="shared" si="4"/>
-        <v>2217</v>
+        <v>2109</v>
       </c>
       <c r="AI8">
         <f t="shared" si="4"/>
-        <v>2587</v>
+        <v>2009</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="4"/>
-        <v>2410</v>
+        <v>2325</v>
       </c>
       <c r="AK8">
         <f t="shared" si="4"/>
-        <v>2591</v>
+        <v>2514</v>
       </c>
       <c r="AL8">
         <f t="shared" si="4"/>
-        <v>2278</v>
+        <v>2286</v>
       </c>
       <c r="AM8">
         <f t="shared" si="4"/>
-        <v>2784</v>
+        <v>2359</v>
       </c>
       <c r="AN8">
         <f t="shared" si="4"/>
-        <v>3066</v>
+        <v>2538</v>
       </c>
       <c r="AO8">
         <f t="shared" si="4"/>
-        <v>3175</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.2">
@@ -4195,7 +5572,7 @@
       </c>
       <c r="Z10" s="34">
         <f>MAX(Z8:AP8)</f>
-        <v>3175</v>
+        <v>2760</v>
       </c>
       <c r="AB10" s="33" t="s">
         <v>40</v>
@@ -4264,14 +5641,14 @@
       </c>
       <c r="Z11" s="34">
         <f>LARGE(Z8:AP8,2)</f>
-        <v>3066</v>
+        <v>2538</v>
       </c>
       <c r="AB11" s="34" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="34" cm="1">
         <f t="array" ref="AC11">INDEX(Z6:AO6,1,Z12+1)+HLOOKUP(INDEX(Z4:AO4,1,AC10+1),$A$20:$R$37,INDEX(Z3:AO3,1,Z12+1)+2)</f>
-        <v>3255</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
@@ -4341,7 +5718,7 @@
       </c>
       <c r="AC12" s="34" cm="1">
         <f t="array" ref="AC12">INDEX(Z6:AO6,1,AC10+1)+HLOOKUP(INDEX(Z4:AO4,1,Z12+1),$A$20:$R$37,INDEX(Z3:AO3,1,AC10+1)+2)</f>
-        <v>1442</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
@@ -4574,54 +5951,6 @@
       <c r="R16">
         <v>153</v>
       </c>
-      <c r="Z16">
-        <v>15</v>
-      </c>
-      <c r="AA16">
-        <v>9</v>
-      </c>
-      <c r="AB16">
-        <v>1</v>
-      </c>
-      <c r="AC16">
-        <v>2</v>
-      </c>
-      <c r="AD16">
-        <v>10</v>
-      </c>
-      <c r="AE16">
-        <v>14</v>
-      </c>
-      <c r="AF16">
-        <v>13</v>
-      </c>
-      <c r="AG16">
-        <v>16</v>
-      </c>
-      <c r="AH16">
-        <v>4</v>
-      </c>
-      <c r="AI16">
-        <v>7</v>
-      </c>
-      <c r="AJ16">
-        <v>6</v>
-      </c>
-      <c r="AK16">
-        <v>12</v>
-      </c>
-      <c r="AL16">
-        <v>3</v>
-      </c>
-      <c r="AM16">
-        <v>8</v>
-      </c>
-      <c r="AN16">
-        <v>11</v>
-      </c>
-      <c r="AO16">
-        <v>5</v>
-      </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -4843,53 +6172,53 @@
       <c r="R21">
         <v>0</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="33">
+        <v>15</v>
+      </c>
+      <c r="AA21" s="33">
+        <v>9</v>
+      </c>
+      <c r="AB21" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="33">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="33">
+        <v>10</v>
+      </c>
+      <c r="AE21" s="33">
+        <v>14</v>
+      </c>
+      <c r="AF21" s="33">
+        <v>13</v>
+      </c>
+      <c r="AG21" s="33">
+        <v>16</v>
+      </c>
+      <c r="AH21" s="33">
+        <v>4</v>
+      </c>
+      <c r="AI21" s="33">
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="33">
+        <v>6</v>
+      </c>
+      <c r="AK21" s="33">
+        <v>12</v>
+      </c>
+      <c r="AL21" s="33">
         <v>3</v>
       </c>
-      <c r="AA21">
-        <v>12</v>
-      </c>
-      <c r="AB21">
-        <v>6</v>
-      </c>
-      <c r="AC21">
-        <v>7</v>
-      </c>
-      <c r="AD21">
+      <c r="AM21" s="33">
+        <v>8</v>
+      </c>
+      <c r="AN21" s="33">
+        <v>11</v>
+      </c>
+      <c r="AO21" s="33">
         <v>5</v>
-      </c>
-      <c r="AE21">
-        <v>16</v>
-      </c>
-      <c r="AF21">
-        <v>13</v>
-      </c>
-      <c r="AG21">
-        <v>14</v>
-      </c>
-      <c r="AH21">
-        <v>2</v>
-      </c>
-      <c r="AI21">
-        <v>10</v>
-      </c>
-      <c r="AJ21">
-        <v>9</v>
-      </c>
-      <c r="AK21">
-        <v>1</v>
-      </c>
-      <c r="AL21">
-        <v>4</v>
-      </c>
-      <c r="AM21">
-        <v>8</v>
-      </c>
-      <c r="AN21">
-        <v>15</v>
-      </c>
-      <c r="AO21">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
@@ -5801,7 +7130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F40EA9-1EC3-0541-AAAB-A8752A20DC08}">
   <dimension ref="A1:V51"/>
   <sheetViews>
@@ -7138,7 +8467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24F2CA6-0EA3-9043-BA16-3F926E06AD85}">
   <dimension ref="A1:J103"/>
   <sheetViews>
@@ -10453,4 +11782,1666 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E956EB-F175-5B46-9D4C-0D0BAB0A425B}">
+  <dimension ref="A1:W27"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="2.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2760</v>
+      </c>
+      <c r="D3">
+        <v>2760</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.1139</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>5.6338310241699201E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>2760</v>
+      </c>
+      <c r="P3">
+        <v>2760</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.1024</v>
+      </c>
+      <c r="S3" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>2.87222862243652E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>7788</v>
+      </c>
+      <c r="D4">
+        <v>7788</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>41</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>2.6543855667114199E-2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>7788</v>
+      </c>
+      <c r="P4">
+        <v>7788</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.37990000000000002</v>
+      </c>
+      <c r="S4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>14</v>
+      </c>
+      <c r="W4">
+        <v>1.06012821197509E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1806</v>
+      </c>
+      <c r="D5">
+        <v>1806</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.19980000000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1.33328437805175E-2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>1806</v>
+      </c>
+      <c r="P5">
+        <v>1806</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.36830000000000002</v>
+      </c>
+      <c r="S5" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>17</v>
+      </c>
+      <c r="W5">
+        <v>1.51162147521972E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1283</v>
+      </c>
+      <c r="D6">
+        <v>1283</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.38179999999999997</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>112</v>
+      </c>
+      <c r="J6">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <v>6.1474323272705002E-2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>1283</v>
+      </c>
+      <c r="P6">
+        <v>1283</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.23219999999999999</v>
+      </c>
+      <c r="S6" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>11</v>
+      </c>
+      <c r="W6">
+        <v>1.12268924713134E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2916</v>
+      </c>
+      <c r="D7">
+        <v>2915.81</v>
+      </c>
+      <c r="E7">
+        <v>6.6E-3</v>
+      </c>
+      <c r="F7">
+        <v>1.8534999999999999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>579</v>
+      </c>
+      <c r="J7">
+        <v>124</v>
+      </c>
+      <c r="K7">
+        <v>0.35060572624206499</v>
+      </c>
+      <c r="M7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>2916</v>
+      </c>
+      <c r="P7">
+        <v>2916</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1.1415</v>
+      </c>
+      <c r="S7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>101</v>
+      </c>
+      <c r="V7">
+        <v>71</v>
+      </c>
+      <c r="W7">
+        <v>9.2331171035766602E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>7282</v>
+      </c>
+      <c r="D8">
+        <v>7281.56</v>
+      </c>
+      <c r="E8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>18.9238</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>2785</v>
+      </c>
+      <c r="J8">
+        <v>442</v>
+      </c>
+      <c r="K8">
+        <v>4.1244804859161297</v>
+      </c>
+      <c r="M8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>7282</v>
+      </c>
+      <c r="P8">
+        <v>7282</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>6.8567</v>
+      </c>
+      <c r="S8" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8">
+        <v>247</v>
+      </c>
+      <c r="V8">
+        <v>195</v>
+      </c>
+      <c r="W8">
+        <v>0.49526762962341297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>628.51</v>
+      </c>
+      <c r="D9">
+        <v>628.51</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2.39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>90</v>
+      </c>
+      <c r="J9">
+        <v>83</v>
+      </c>
+      <c r="K9">
+        <v>0.26506233215331998</v>
+      </c>
+      <c r="M9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9">
+        <v>628.51</v>
+      </c>
+      <c r="P9">
+        <v>628.51</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>3.1821999999999999</v>
+      </c>
+      <c r="S9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>141</v>
+      </c>
+      <c r="V9">
+        <v>129</v>
+      </c>
+      <c r="W9">
+        <v>0.41895580291748002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>11087.21</v>
+      </c>
+      <c r="D10">
+        <v>11086.38</v>
+      </c>
+      <c r="E10">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F10">
+        <v>4.6406000000000001</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>314</v>
+      </c>
+      <c r="J10">
+        <v>157</v>
+      </c>
+      <c r="K10">
+        <v>0.66410350799560502</v>
+      </c>
+      <c r="M10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10">
+        <v>11087.21</v>
+      </c>
+      <c r="P10">
+        <v>11087.21</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>4.2591000000000001</v>
+      </c>
+      <c r="S10" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>119</v>
+      </c>
+      <c r="V10">
+        <v>107</v>
+      </c>
+      <c r="W10">
+        <v>0.34116077423095698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>801.91</v>
+      </c>
+      <c r="D11">
+        <v>801.86</v>
+      </c>
+      <c r="E11">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="F11">
+        <v>14.946099999999999</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>705</v>
+      </c>
+      <c r="J11">
+        <v>463</v>
+      </c>
+      <c r="K11">
+        <v>3.23772740364074</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11">
+        <v>801.91</v>
+      </c>
+      <c r="P11">
+        <v>801.91</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>10.080500000000001</v>
+      </c>
+      <c r="S11" t="s">
+        <v>56</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11">
+        <v>113</v>
+      </c>
+      <c r="V11">
+        <v>113</v>
+      </c>
+      <c r="W11">
+        <v>0.70464849472045898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>945.32</v>
+      </c>
+      <c r="D12">
+        <v>945.27</v>
+      </c>
+      <c r="E12">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F12">
+        <v>39.839300000000001</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>1193</v>
+      </c>
+      <c r="J12">
+        <v>359</v>
+      </c>
+      <c r="K12">
+        <v>8.4108557701110804</v>
+      </c>
+      <c r="M12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12">
+        <v>945.32</v>
+      </c>
+      <c r="P12">
+        <v>945.32</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>24.297499999999999</v>
+      </c>
+      <c r="S12" t="s">
+        <v>56</v>
+      </c>
+      <c r="T12">
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <v>505</v>
+      </c>
+      <c r="V12">
+        <v>327</v>
+      </c>
+      <c r="W12">
+        <v>3.9928278923034601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
+        <v>3729.7950000000005</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3729.6390000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="F13" s="42">
+        <f>AVERAGE(F3:F12)</f>
+        <v>8.3736999999999995</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13" si="1">AVERAGE(H3:H12)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I13" s="42">
+        <f t="shared" ref="I13" si="2">AVERAGE(I3:I12)</f>
+        <v>582.29999999999995</v>
+      </c>
+      <c r="J13" s="42">
+        <f t="shared" ref="J13:K13" si="3">AVERAGE(J3:J12)</f>
+        <v>167.3</v>
+      </c>
+      <c r="K13" s="42">
+        <f t="shared" si="3"/>
+        <v>1.7159820079803445</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13" si="4">AVERAGE(O3:O12)</f>
+        <v>3729.7950000000005</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13" si="5">AVERAGE(P3:P12)</f>
+        <v>3729.7950000000005</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13" si="6">AVERAGE(Q3:Q12)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="42">
+        <f t="shared" ref="R13" si="7">AVERAGE(R3:R12)</f>
+        <v>5.0900300000000005</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13" si="8">AVERAGE(T3:T12)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="U13" s="42">
+        <f t="shared" ref="U13" si="9">AVERAGE(U3:U12)</f>
+        <v>123</v>
+      </c>
+      <c r="V13" s="42">
+        <f t="shared" ref="V13" si="10">AVERAGE(V3:V12)</f>
+        <v>98.7</v>
+      </c>
+      <c r="W13" s="42">
+        <f t="shared" ref="W13" si="11">AVERAGE(W3:W12)</f>
+        <v>0.60850083827972345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>49</v>
+      </c>
+      <c r="R16" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" t="s">
+        <v>50</v>
+      </c>
+      <c r="T16" t="s">
+        <v>51</v>
+      </c>
+      <c r="U16" t="s">
+        <v>52</v>
+      </c>
+      <c r="V16" t="s">
+        <v>53</v>
+      </c>
+      <c r="W16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>2760</v>
+      </c>
+      <c r="D17">
+        <v>2760</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.16189999999999999</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>6.1836242675781198E-3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17">
+        <v>2760</v>
+      </c>
+      <c r="P17">
+        <v>2760</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0.1409</v>
+      </c>
+      <c r="S17" t="s">
+        <v>56</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>4</v>
+      </c>
+      <c r="W17">
+        <v>4.0507316589355399E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>7788</v>
+      </c>
+      <c r="D18">
+        <v>7788</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0.54920000000000002</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>4.1981697082519497E-2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18">
+        <v>7788</v>
+      </c>
+      <c r="P18">
+        <v>7788</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0.53580000000000005</v>
+      </c>
+      <c r="S18" t="s">
+        <v>56</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>15</v>
+      </c>
+      <c r="W18">
+        <v>3.3878564834594699E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1806</v>
+      </c>
+      <c r="D19">
+        <v>1806</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.67589999999999995</v>
+      </c>
+      <c r="G19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>12</v>
+      </c>
+      <c r="K19">
+        <v>6.5450191497802707E-2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19">
+        <v>1806</v>
+      </c>
+      <c r="P19">
+        <v>1806</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0.6573</v>
+      </c>
+      <c r="S19" t="s">
+        <v>56</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>12</v>
+      </c>
+      <c r="W19">
+        <v>5.7492733001708901E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>1283</v>
+      </c>
+      <c r="D20">
+        <v>1283</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+      <c r="K20">
+        <v>0.12560534477233801</v>
+      </c>
+      <c r="M20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20">
+        <v>1283</v>
+      </c>
+      <c r="P20">
+        <v>1283</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0.62260000000000004</v>
+      </c>
+      <c r="S20" t="s">
+        <v>56</v>
+      </c>
+      <c r="T20">
+        <v>2</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>13</v>
+      </c>
+      <c r="W20">
+        <v>0.117739677429199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>2916</v>
+      </c>
+      <c r="D21">
+        <v>2916</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2.8771</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <v>21</v>
+      </c>
+      <c r="J21">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>0.21608233451843201</v>
+      </c>
+      <c r="M21" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21">
+        <v>2916</v>
+      </c>
+      <c r="P21">
+        <v>2916</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>2.8121</v>
+      </c>
+      <c r="S21" t="s">
+        <v>56</v>
+      </c>
+      <c r="T21">
+        <v>6</v>
+      </c>
+      <c r="U21">
+        <v>21</v>
+      </c>
+      <c r="V21">
+        <v>25</v>
+      </c>
+      <c r="W21">
+        <v>0.19626951217651301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>7282</v>
+      </c>
+      <c r="D22">
+        <v>7282</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>7.6454000000000004</v>
+      </c>
+      <c r="G22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>41</v>
+      </c>
+      <c r="J22">
+        <v>33</v>
+      </c>
+      <c r="K22">
+        <v>0.56039547920226995</v>
+      </c>
+      <c r="M22" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22">
+        <v>7282</v>
+      </c>
+      <c r="P22">
+        <v>7282</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>7.5345000000000004</v>
+      </c>
+      <c r="S22" t="s">
+        <v>56</v>
+      </c>
+      <c r="T22">
+        <v>6</v>
+      </c>
+      <c r="U22">
+        <v>41</v>
+      </c>
+      <c r="V22">
+        <v>33</v>
+      </c>
+      <c r="W22">
+        <v>0.499192714691162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>628.51</v>
+      </c>
+      <c r="D23">
+        <v>628.51</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>7.5723000000000003</v>
+      </c>
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23">
+        <v>6</v>
+      </c>
+      <c r="I23">
+        <v>55</v>
+      </c>
+      <c r="J23">
+        <v>26</v>
+      </c>
+      <c r="K23">
+        <v>0.428300380706787</v>
+      </c>
+      <c r="M23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23">
+        <v>628.51</v>
+      </c>
+      <c r="P23">
+        <v>628.51</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>7.4947999999999997</v>
+      </c>
+      <c r="S23" t="s">
+        <v>56</v>
+      </c>
+      <c r="T23">
+        <v>6</v>
+      </c>
+      <c r="U23">
+        <v>55</v>
+      </c>
+      <c r="V23">
+        <v>26</v>
+      </c>
+      <c r="W23">
+        <v>0.379902124404907</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>11087.21</v>
+      </c>
+      <c r="D24">
+        <v>11087.21</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>7.0952000000000002</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
+      </c>
+      <c r="J24">
+        <v>36</v>
+      </c>
+      <c r="K24">
+        <v>0.69217395782470703</v>
+      </c>
+      <c r="M24" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24">
+        <v>11087.21</v>
+      </c>
+      <c r="P24">
+        <v>11087.21</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>6.8855000000000004</v>
+      </c>
+      <c r="S24" t="s">
+        <v>56</v>
+      </c>
+      <c r="T24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <v>31</v>
+      </c>
+      <c r="V24">
+        <v>36</v>
+      </c>
+      <c r="W24">
+        <v>0.591455698013305</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>801.91</v>
+      </c>
+      <c r="D25">
+        <v>801.89</v>
+      </c>
+      <c r="E25">
+        <v>2.3E-3</v>
+      </c>
+      <c r="F25">
+        <v>15.9933</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>37</v>
+      </c>
+      <c r="J25">
+        <v>42</v>
+      </c>
+      <c r="K25">
+        <v>1.4338083267211901</v>
+      </c>
+      <c r="M25" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25">
+        <v>801.91</v>
+      </c>
+      <c r="P25">
+        <v>801.89</v>
+      </c>
+      <c r="Q25">
+        <v>2.3E-3</v>
+      </c>
+      <c r="R25">
+        <v>15.6496</v>
+      </c>
+      <c r="S25" t="s">
+        <v>56</v>
+      </c>
+      <c r="T25">
+        <v>4</v>
+      </c>
+      <c r="U25">
+        <v>37</v>
+      </c>
+      <c r="V25">
+        <v>42</v>
+      </c>
+      <c r="W25">
+        <v>1.2026386260986299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>945.32</v>
+      </c>
+      <c r="D26">
+        <v>945.23</v>
+      </c>
+      <c r="E26">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F26">
+        <v>106.435</v>
+      </c>
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>218</v>
+      </c>
+      <c r="J26">
+        <v>122</v>
+      </c>
+      <c r="K26">
+        <v>14.065950393676699</v>
+      </c>
+      <c r="M26" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26">
+        <v>945.32</v>
+      </c>
+      <c r="P26">
+        <v>945.23</v>
+      </c>
+      <c r="Q26">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="R26">
+        <v>103.5599</v>
+      </c>
+      <c r="S26" t="s">
+        <v>56</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
+      </c>
+      <c r="U26">
+        <v>218</v>
+      </c>
+      <c r="V26">
+        <v>122</v>
+      </c>
+      <c r="W26">
+        <v>12.908519744873001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f>AVERAGE(C17:C26)</f>
+        <v>3729.7950000000005</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27" si="12">AVERAGE(D17:D26)</f>
+        <v>3729.7840000000006</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27" si="13">AVERAGE(E17:E26)</f>
+        <v>1.1899999999999999E-3</v>
+      </c>
+      <c r="F27" s="42">
+        <f t="shared" ref="F27" si="14">AVERAGE(F17:F26)</f>
+        <v>14.96433</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27" si="15">AVERAGE(H17:H26)</f>
+        <v>4.2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27" si="16">AVERAGE(I17:I26)</f>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27" si="17">AVERAGE(J17:J26)</f>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27" si="18">AVERAGE(K17:K26)</f>
+        <v>1.7635931730270322</v>
+      </c>
+      <c r="O27">
+        <f>AVERAGE(O17:O26)</f>
+        <v>3729.7950000000005</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ref="P27:W27" si="19">AVERAGE(P17:P26)</f>
+        <v>3729.7840000000006</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="19"/>
+        <v>1.1899999999999999E-3</v>
+      </c>
+      <c r="R27" s="42">
+        <f t="shared" si="19"/>
+        <v>14.5893</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="19"/>
+        <v>4.2</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="19"/>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="19"/>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="19"/>
+        <v>1.5991140127181955</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>